<commit_message>
Excel file updated to include 3 detectors results
</commit_message>
<xml_diff>
--- a/BasicResultGraph.xlsx
+++ b/BasicResultGraph.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Documents\Project\DetectorEstimator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Documents\Projects\DetectorEstimator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,11 +23,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Patrick Cooper</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Patrick Cooper:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Low on account of high frame rate of capture most likely. However, I do not believe this will hold up with worse imagry where more specific detail is tracked.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Patrick Cooper:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This take FAST out of the running as best feature detector as it will be sensitive to glare and other image artifacts.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
-  <si>
-    <t>Detectors</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>SURF</t>
   </si>
@@ -50,29 +105,52 @@
     <t>Speed Per Keypoint</t>
   </si>
   <si>
-    <t>Percent of Tracked Features</t>
-  </si>
-  <si>
-    <t>Features Count Deviation (Looks at exposure)</t>
-  </si>
-  <si>
     <t>Detector</t>
   </si>
   <si>
     <t>Feature Count Deviation (response to exposure)</t>
+  </si>
+  <si>
+    <t>Tracked Features Preserved (successful point transfer)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,8 +173,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,6 +191,1151 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Feature</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Detector Comparison on Space Object (No Glare)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speed Per Frame</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>SURF</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FAST</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SIFT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>STAR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MSER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.15599989891052199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0999898910522398E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.2999963760375893E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A1F-4516-9875-0AF67209FB02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speed Per Keypoint</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>SURF</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FAST</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SIFT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>STAR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MSER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1.0399993260701399E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0558549927216205E-7</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>3.7058802211985798E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3A1F-4516-9875-0AF67209FB02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tracked Features Preserved (successful point transfer)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>SURF</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FAST</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SIFT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>STAR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MSER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3A1F-4516-9875-0AF67209FB02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Feature Count Deviation (response to exposure)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>SURF</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FAST</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SIFT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>STAR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MSER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3A1F-4516-9875-0AF67209FB02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="431878856"/>
+        <c:axId val="431879184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="431878856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431879184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="431879184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="431878856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE33900-7D7C-4CA9-BD29-850939B37090}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,11 +1634,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,89 +1655,86 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.15599989891052199</v>
+      </c>
+      <c r="C2">
+        <v>1.0399993260701399E-2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3.0999898910522398E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>7.0558549927216205E-7</v>
+      </c>
+      <c r="D3">
         <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
+      <c r="B6">
+        <v>6.2999963760375893E-2</v>
+      </c>
+      <c r="C6">
+        <v>3.7058802211985798E-3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>